<commit_message>
Separated test files from training.
</commit_message>
<xml_diff>
--- a/data/Uber.xlsx
+++ b/data/Uber.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbookpro/Documents/Git/Projeto2/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos Dip\Repos\BayesianSentimentAnalyzer\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{836F6485-E640-9A49-9D4F-5C8E2F4A06A2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82323DFF-6741-4662-9671-FE86C0C291E6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -2037,7 +2037,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2357,19 +2357,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D301"/>
+  <dimension ref="A1:D401"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" topLeftCell="A356" workbookViewId="0">
+      <selection activeCell="B302" sqref="B302"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="111" style="2" customWidth="1"/>
     <col min="2" max="2" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2383,7 +2383,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -2391,7 +2391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -2399,7 +2399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -2407,7 +2407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -2415,7 +2415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -2423,7 +2423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -2431,7 +2431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -2439,7 +2439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -2447,7 +2447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -2455,7 +2455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -2463,7 +2463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
@@ -2471,7 +2471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -2479,7 +2479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -2487,7 +2487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -2495,7 +2495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -2503,7 +2503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
@@ -2511,7 +2511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
@@ -2519,7 +2519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
@@ -2527,7 +2527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
@@ -2535,7 +2535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
@@ -2543,7 +2543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
@@ -2551,7 +2551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="64" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
@@ -2559,7 +2559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
@@ -2567,7 +2567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>24</v>
       </c>
@@ -2575,7 +2575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>25</v>
       </c>
@@ -2583,7 +2583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>26</v>
       </c>
@@ -2591,7 +2591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
@@ -2599,7 +2599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>28</v>
       </c>
@@ -2607,7 +2607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
@@ -2615,7 +2615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>30</v>
       </c>
@@ -2623,7 +2623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="48" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>31</v>
       </c>
@@ -2631,7 +2631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>32</v>
       </c>
@@ -2639,7 +2639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>33</v>
       </c>
@@ -2647,7 +2647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>34</v>
       </c>
@@ -2655,7 +2655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>35</v>
       </c>
@@ -2663,7 +2663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>36</v>
       </c>
@@ -2671,7 +2671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>37</v>
       </c>
@@ -2679,7 +2679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>38</v>
       </c>
@@ -2687,7 +2687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>39</v>
       </c>
@@ -2695,7 +2695,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>40</v>
       </c>
@@ -2703,7 +2703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>41</v>
       </c>
@@ -2711,7 +2711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>42</v>
       </c>
@@ -2719,7 +2719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>43</v>
       </c>
@@ -2727,7 +2727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>44</v>
       </c>
@@ -2735,7 +2735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>45</v>
       </c>
@@ -2743,7 +2743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>46</v>
       </c>
@@ -2751,1274 +2751,1774 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:1" ht="48" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:1" ht="48" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:1" ht="64" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="107" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="108" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="109" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="110" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="111" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="112" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="113" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="114" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="115" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="116" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="117" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="118" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="119" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="120" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="121" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="122" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="123" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="124" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="125" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="126" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="127" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="128" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="129" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="130" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="131" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="132" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="133" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="134" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="135" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="136" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="137" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="138" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="139" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="140" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="141" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="142" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="143" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="144" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="145" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="146" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="147" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="148" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A148" s="2" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="149" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A149" s="2" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="150" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A150" s="2" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="151" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A151" s="2" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="152" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="153" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A153" s="2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="154" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A154" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="155" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A155" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="156" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A156" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="157" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A157" s="2" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="158" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A158" s="2" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="159" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A159" s="2" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="160" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A160" s="2" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="161" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A161" s="2" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="162" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A162" s="2" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="163" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A163" s="2" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="164" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A164" s="2" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="165" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A165" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="166" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A166" s="2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="167" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A167" s="2" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="168" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A168" s="2" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="169" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A169" s="2" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="170" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A170" s="2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="171" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A171" s="2" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="172" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A172" s="2" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="173" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A173" s="2" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="174" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A174" s="2" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="175" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A175" s="2" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="176" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A176" s="2" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="177" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A177" s="2" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="178" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A178" s="2" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="179" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A179" s="2" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="180" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A180" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="181" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A181" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="182" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A182" s="2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="183" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A183" s="2" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="184" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A184" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="185" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A185" s="2" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="186" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A186" s="2" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="187" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A187" s="2" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="188" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A188" s="2" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="189" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A189" s="2" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="190" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A190" s="2" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="191" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A191" s="2" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="192" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A192" s="2" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="193" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A193" s="2" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="194" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A194" s="2" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="195" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A195" s="2" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="196" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A196" s="2" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="197" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A197" s="2" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="198" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A198" s="2" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="199" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A199" s="2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="200" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A200" s="2" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="201" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A201" s="2" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="202" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A202" s="2" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="203" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A203" s="2" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="204" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A204" s="2" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="205" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A205" s="2" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="206" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A206" s="2" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="207" spans="1:1" ht="48" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A207" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="208" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A208" s="2" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="209" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A209" s="2" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="210" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A210" s="2" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="211" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A211" s="2" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="212" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A212" s="2" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="213" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A213" s="2" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="214" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A214" s="2" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="215" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A215" s="2" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="216" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A216" s="2" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="217" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A217" s="2" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="218" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A218" s="2" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="219" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A219" s="2" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="220" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A220" s="2" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="221" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A221" s="2" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="222" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A222" s="2" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="223" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A223" s="2" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="224" spans="1:1" ht="48" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A224" s="2" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="225" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A225" s="2" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="226" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A226" s="2" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="227" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A227" s="2" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="228" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A228" s="2" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="229" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A229" s="2" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="230" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A230" s="2" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="231" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A231" s="2" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="232" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A232" s="2" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="233" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A233" s="2" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="234" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A234" s="2" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="235" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A235" s="2" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="236" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A236" s="2" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="237" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A237" s="2" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="238" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A238" s="2" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="239" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A239" s="2" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="240" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A240" s="2" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="241" spans="1:1" ht="48" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A241" s="2" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="242" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A242" s="2" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="243" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A243" s="2" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="244" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A244" s="2" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="245" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A245" s="2" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="246" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A246" s="2" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="247" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A247" s="2" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="248" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A248" s="2" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="249" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A249" s="2" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="250" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A250" s="2" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="251" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A251" s="2" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="252" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A252" s="2" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="253" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A253" s="2" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="254" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A254" s="2" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="255" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A255" s="2" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="256" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A256" s="2" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="257" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A257" s="2" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="258" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A258" s="2" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="259" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A259" s="2" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="260" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A260" s="2" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="261" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A261" s="2" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="262" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A262" s="2" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="263" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A263" s="2" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="264" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A264" s="2" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="265" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A265" s="2" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="266" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A266" s="2" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="267" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A267" s="2" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="268" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A268" s="2" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="269" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A269" s="2" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="270" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A270" s="2" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="271" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A271" s="2" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="272" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A272" s="2" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="273" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A273" s="2" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="274" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A274" s="2" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="275" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A275" s="2" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="276" spans="1:1" ht="48" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A276" s="2" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="277" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A277" s="2" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="278" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A278" s="2" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="279" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A279" s="2" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="280" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A280" s="2" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="281" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A281" s="2" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="282" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A282" s="2" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="283" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A283" s="2" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="284" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A284" s="2" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="285" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A285" s="2" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="286" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A286" s="2" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="287" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A287" s="2" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="288" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A288" s="2" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="289" spans="1:1" ht="80" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:1" ht="72" x14ac:dyDescent="0.3">
       <c r="A289" s="2" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="290" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A290" s="2" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="291" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A291" s="2" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="292" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A292" s="2" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="293" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A293" s="2" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="294" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A294" s="2" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="295" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A295" s="2" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="296" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A296" s="2" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="297" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A297" s="2" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="298" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A298" s="2" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="299" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A299" s="2" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="300" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A300" s="2" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="301" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A301" s="2" t="s">
         <v>300</v>
+      </c>
+    </row>
+    <row r="302" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A302" s="2" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="303" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A303" s="2" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="304" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A304" s="2" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="305" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A305" s="2" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="306" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A306" s="2" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="307" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A307" s="2" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="308" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A308" s="2" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="309" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A309" s="2" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="310" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A310" s="2" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="311" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A311" s="2" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="312" spans="1:1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A312" s="2" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="313" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A313" s="2" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="314" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A314" s="2" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="315" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A315" s="2" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="316" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A316" s="2" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="317" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A317" s="2" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="318" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A318" s="2" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="319" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A319" s="2" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="320" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A320" s="2" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="321" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A321" s="2" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="322" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A322" s="2" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="323" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A323" s="2" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="324" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A324" s="2" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="325" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A325" s="2" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="326" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A326" s="2" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="327" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A327" s="2" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="328" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A328" s="2" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="329" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A329" s="2" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="330" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A330" s="2" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="331" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A331" s="2" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="332" spans="1:1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A332" s="2" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="333" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A333" s="2" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="334" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A334" s="2" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="335" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A335" s="2" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="336" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A336" s="2" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="337" spans="1:1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A337" s="2" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="338" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A338" s="2" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="339" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A339" s="2" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="340" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A340" s="2" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="341" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A341" s="2" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="342" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A342" s="2" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="343" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A343" s="2" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="344" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A344" s="2" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="345" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A345" s="2" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="346" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A346" s="2" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="347" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A347" s="2" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="348" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A348" s="2" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="349" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A349" s="2" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="350" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A350" s="2" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="351" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A351" s="2" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="352" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A352" s="2" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="353" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A353" s="2" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="354" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A354" s="2" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="355" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A355" s="2" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="356" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A356" s="2" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="357" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A357" s="2" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="358" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A358" s="2" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="359" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A359" s="2" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="360" spans="1:1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A360" s="2" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="361" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A361" s="2" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="362" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A362" s="2" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="363" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A363" s="2" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="364" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A364" s="2" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="365" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A365" s="2" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="366" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A366" s="2" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="367" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A367" s="2" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="368" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A368" s="2" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="369" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A369" s="2" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="370" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A370" s="2" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="371" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A371" s="2" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="372" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A372" s="2" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="373" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A373" s="2" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="374" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A374" s="2" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="375" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A375" s="2" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="376" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A376" s="2" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="377" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A377" s="2" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="378" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A378" s="2" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="379" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A379" s="2" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="380" spans="1:1" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A380" s="2" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="381" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A381" s="2" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="382" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A382" s="2" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="383" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A383" s="2" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="384" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A384" s="2" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="385" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A385" s="2" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="386" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A386" s="2" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="387" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A387" s="2" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="388" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A388" s="2" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="389" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A389" s="2" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="390" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A390" s="2" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="391" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A391" s="2" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="392" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A392" s="2" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="393" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A393" s="2" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="394" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A394" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="395" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A395" s="2" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="396" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A396" s="2" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="397" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A397" s="2" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="398" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A398" s="2" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="399" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A399" s="2" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="400" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A400" s="2" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="401" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A401" s="2" t="s">
+        <v>600</v>
       </c>
     </row>
   </sheetData>
@@ -4028,19 +4528,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B300"/>
+  <dimension ref="A1:B200"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="A287" workbookViewId="0">
+      <selection activeCell="A300" sqref="A201:A300"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="88.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="10.1640625" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>301</v>
       </c>
@@ -4048,1499 +4548,999 @@
         <v>602</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="48" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="80" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" ht="72" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="26" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="27" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="28" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="29" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="30" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="31" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="32" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="33" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="34" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="36" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="37" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="38" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="39" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="40" spans="1:1" ht="144" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="41" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="42" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="43" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="44" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="45" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="46" spans="1:1" ht="96" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="47" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="48" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="49" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="50" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="51" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="52" spans="1:1" ht="48" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="53" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="54" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="55" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="56" spans="1:1" ht="80" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1" ht="72" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="57" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="58" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="59" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="60" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="61" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="62" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="63" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="64" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="65" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="66" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="67" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="68" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="69" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="70" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="71" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="72" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="73" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="74" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="75" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="76" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="77" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="78" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="79" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="80" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="81" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="82" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="83" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="84" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="85" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="86" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="87" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="88" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="89" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="90" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="91" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="92" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="93" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="94" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="95" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="96" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="97" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="98" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="99" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="100" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="101" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="102" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="103" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="104" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="105" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="106" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="107" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="108" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="109" spans="1:1" ht="48" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="110" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="111" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="112" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="113" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="114" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="115" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="116" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="117" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="118" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="119" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="120" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="121" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="122" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="123" spans="1:1" ht="48" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="124" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="125" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="126" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="127" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="128" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="129" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="130" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="131" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="132" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="133" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="134" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="135" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="136" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="137" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="138" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="139" spans="1:1" ht="48" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="140" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="141" spans="1:1" ht="80" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:1" ht="72" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="142" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="143" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="144" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="145" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="146" spans="1:1" ht="48" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="147" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="148" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A148" s="2" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="149" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A149" s="2" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="150" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A150" s="2" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="151" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A151" s="2" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="152" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="153" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A153" s="2" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="154" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A154" s="2" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="155" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A155" s="2" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="156" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A156" s="2" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="157" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A157" s="2" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="158" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A158" s="2" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="159" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A159" s="2" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="160" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A160" s="2" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="161" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A161" s="2" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="162" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A162" s="2" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="163" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A163" s="2" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="164" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A164" s="2" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="165" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A165" s="2" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="166" spans="1:1" ht="80" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:1" ht="72" x14ac:dyDescent="0.3">
       <c r="A166" s="2" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="167" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A167" s="2" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="168" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A168" s="2" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="169" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A169" s="2" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="170" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A170" s="2" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="171" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A171" s="2" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="172" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A172" s="2" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="173" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A173" s="2" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="174" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A174" s="2" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="175" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A175" s="2" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="176" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A176" s="2" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="177" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A177" s="2" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="178" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A178" s="2" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="179" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A179" s="2" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="180" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A180" s="2" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="181" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A181" s="2" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="182" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A182" s="2" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="183" spans="1:1" ht="80" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:1" ht="72" x14ac:dyDescent="0.3">
       <c r="A183" s="2" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="184" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A184" s="2" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="185" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A185" s="2" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="186" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A186" s="2" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="187" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A187" s="2" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="188" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A188" s="2" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="189" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A189" s="2" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="190" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A190" s="2" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="191" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A191" s="2" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="192" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A192" s="2" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="193" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A193" s="2" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="194" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A194" s="2" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="195" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A195" s="2" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="196" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A196" s="2" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="197" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A197" s="2" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="198" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A198" s="2" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="199" spans="1:1" ht="80" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:1" ht="72" x14ac:dyDescent="0.3">
       <c r="A199" s="2" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="200" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A200" s="2" t="s">
         <v>500</v>
-      </c>
-    </row>
-    <row r="201" spans="1:1" ht="80" x14ac:dyDescent="0.2">
-      <c r="A201" s="2" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="202" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A202" s="2" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="203" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A203" s="2" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="204" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A204" s="2" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="205" spans="1:1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A205" s="2" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="206" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A206" s="2" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="207" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A207" s="2" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="208" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A208" s="2" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="209" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A209" s="2" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="210" spans="1:1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A210" s="2" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="211" spans="1:1" ht="64" x14ac:dyDescent="0.2">
-      <c r="A211" s="2" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="212" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A212" s="2" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="213" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A213" s="2" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="214" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A214" s="2" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="215" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A215" s="2" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="216" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A216" s="2" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="217" spans="1:1" ht="64" x14ac:dyDescent="0.2">
-      <c r="A217" s="2" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="218" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A218" s="2" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="219" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A219" s="2" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="220" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A220" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="221" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A221" s="2" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="222" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A222" s="2" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="223" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A223" s="2" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="224" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A224" s="2" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="225" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A225" s="2" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="226" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A226" s="2" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="227" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A227" s="2" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="228" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A228" s="2" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="229" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A229" s="2" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="230" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A230" s="2" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="231" spans="1:1" ht="80" x14ac:dyDescent="0.2">
-      <c r="A231" s="2" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="232" spans="1:1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A232" s="2" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="233" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A233" s="2" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="234" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A234" s="2" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="235" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A235" s="2" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="236" spans="1:1" ht="80" x14ac:dyDescent="0.2">
-      <c r="A236" s="2" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="237" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A237" s="2" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="238" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A238" s="2" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="239" spans="1:1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A239" s="2" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="240" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A240" s="2" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="241" spans="1:1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A241" s="2" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="242" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A242" s="2" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="243" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A243" s="2" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="244" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A244" s="2" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="245" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A245" s="2" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="246" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A246" s="2" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="247" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A247" s="2" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="248" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A248" s="2" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="249" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A249" s="2" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="250" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A250" s="2" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="251" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A251" s="2" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="252" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A252" s="2" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="253" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A253" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="254" spans="1:1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A254" s="2" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="255" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A255" s="2" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="256" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A256" s="2" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="257" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A257" s="2" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="258" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A258" s="2" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="259" spans="1:1" ht="80" x14ac:dyDescent="0.2">
-      <c r="A259" s="2" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="260" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A260" s="2" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="261" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A261" s="2" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="262" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A262" s="2" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="263" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A263" s="2" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="264" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A264" s="2" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="265" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A265" s="2" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="266" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A266" s="2" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="267" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A267" s="2" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="268" spans="1:1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A268" s="2" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="269" spans="1:1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A269" s="2" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="270" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A270" s="2" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="271" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A271" s="2" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="272" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A272" s="2" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="273" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A273" s="2" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="274" spans="1:1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A274" s="2" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="275" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A275" s="2" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="276" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A276" s="2" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="277" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A277" s="2" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="278" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A278" s="2" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="279" spans="1:1" ht="144" x14ac:dyDescent="0.2">
-      <c r="A279" s="2" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="280" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A280" s="2" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="281" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A281" s="2" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="282" spans="1:1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A282" s="2" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="283" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A283" s="2" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="284" spans="1:1" ht="96" x14ac:dyDescent="0.2">
-      <c r="A284" s="2" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="285" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A285" s="2" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="286" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A286" s="2" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="287" spans="1:1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A287" s="2" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="288" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A288" s="2" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="289" spans="1:1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A289" s="2" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="290" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A290" s="2" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="291" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A291" s="2" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="292" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A292" s="2" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="293" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A293" s="2" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="294" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A294" s="2" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="295" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A295" s="2" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="296" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A296" s="2" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="297" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A297" s="2" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="298" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A298" s="2" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="299" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A299" s="2" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="300" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A300" s="2" t="s">
-        <v>600</v>
       </c>
     </row>
   </sheetData>

</xml_diff>